<commit_message>
backing up definitions after change
</commit_message>
<xml_diff>
--- a/list of definitions.xlsx
+++ b/list of definitions.xlsx
@@ -32,7 +32,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Agrochemical use instead of mix.
 Be explicit about the amount and that it is over a season.</t>
@@ -46,7 +45,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Is legislated the right word?
 - Holding periods
@@ -64,7 +62,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Keep it as simple as possible and aligned with the SWA goals</t>
         </r>
@@ -77,7 +74,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Its not always regional</t>
         </r>
@@ -90,7 +86,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Emphasise that it is the total passes for a whole season</t>
         </r>
@@ -190,7 +185,7 @@
     <t xml:space="preserve">Grape Price</t>
   </si>
   <si>
-    <t xml:space="preserve">The regional grape price of a vineyard</t>
+    <t xml:space="preserve">Grape price per tonne</t>
   </si>
   <si>
     <t xml:space="preserve">Impact on Vine and Vineyard Sward Vigour</t>
@@ -307,7 +302,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -330,7 +324,6 @@
       <sz val="12"/>
       <name val="Liberation Serif;Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -338,13 +331,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Liberation Serif;Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -352,7 +343,6 @@
       <color rgb="FFC9211E"/>
       <name val="Liberation Serif;Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -360,21 +350,18 @@
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Liberation Serif;Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -536,10 +523,10 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="116.85"/>

</xml_diff>